<commit_message>
se implemento la importacion de contactos
</commit_message>
<xml_diff>
--- a/public/uploads/import/contacto.xlsx
+++ b/public/uploads/import/contacto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\atenun_system\public\uploads\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB482D3-9197-4A44-ADBB-1E03E570DE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA635C9-F981-4343-BA30-1FF6452E3E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="1695" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <r>
       <t xml:space="preserve"> </t>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>FORMATO PARA CONTACTO DE PACIENTES</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
   </si>
 </sst>
 </file>
@@ -180,20 +183,20 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +507,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,12 +530,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -540,23 +543,23 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="6"/>
@@ -583,13 +586,15 @@
       <c r="F11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="J11" s="2"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -606,16 +611,16 @@
       <c r="T12" s="7"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H14" s="14"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H15" s="14"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="14"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G19" s="14"/>
+      <c r="G19" s="11"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -625,6 +630,6 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>